<commit_message>
aula 15 do 8 ano
</commit_message>
<xml_diff>
--- a/robotica/Arquivos/img/atividades3tri2024.xlsx
+++ b/robotica/Arquivos/img/atividades3tri2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/23ea03c13864f996/daniloLimaComp/profdanilo.com.br/robotica/Arquivos/img/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="144" documentId="11_F25DC773A252ABDACC10480341994DF85ADE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9EFE81EB-46AA-423F-8B3C-91E557CDE815}"/>
+  <xr:revisionPtr revIDLastSave="145" documentId="11_F25DC773A252ABDACC10480341994DF85ADE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55CD9438-49CF-4EE4-B84B-9BB86BE73609}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3465" windowWidth="28800" windowHeight="11295" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="6 ano" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>Atividade</t>
   </si>
@@ -316,6 +316,12 @@
     <xf numFmtId="16" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -326,12 +332,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="4" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1383,8 +1383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C5351AA-6B27-4E59-98AD-11C7A990BB4F}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A30" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1526,10 +1526,10 @@
     </row>
     <row r="32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C33" s="14"/>
+      <c r="C33" s="16"/>
       <c r="D33" s="6" t="s">
         <v>7</v>
       </c>
@@ -1544,7 +1544,7 @@
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="17" t="s">
         <v>3</v>
       </c>
       <c r="C34" s="2" t="s">
@@ -1554,7 +1554,7 @@
         <v>45565</v>
       </c>
       <c r="E34" s="3">
-        <v>45551</v>
+        <v>45565</v>
       </c>
       <c r="F34" s="3">
         <v>45548</v>
@@ -1564,7 +1564,7 @@
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="15"/>
+      <c r="B35" s="17"/>
       <c r="C35" s="4" t="s">
         <v>2</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>45579</v>
       </c>
       <c r="E35" s="5">
-        <v>45565</v>
+        <v>45579</v>
       </c>
       <c r="F35" s="5">
         <v>45569</v>
@@ -1582,7 +1582,7 @@
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="17" t="s">
         <v>5</v>
       </c>
       <c r="C36" s="2" t="s">
@@ -1592,7 +1592,7 @@
         <v>45579</v>
       </c>
       <c r="E36" s="3">
-        <v>45565</v>
+        <v>45579</v>
       </c>
       <c r="F36" s="3">
         <v>45569</v>
@@ -1602,7 +1602,7 @@
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="15"/>
+      <c r="B37" s="17"/>
       <c r="C37" s="4" t="s">
         <v>2</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>45593</v>
       </c>
       <c r="E37" s="5">
-        <v>45579</v>
+        <v>45593</v>
       </c>
       <c r="F37" s="5">
         <v>45576</v>
@@ -1620,7 +1620,7 @@
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="15" t="s">
+      <c r="B38" s="17" t="s">
         <v>6</v>
       </c>
       <c r="C38" s="2" t="s">
@@ -1630,7 +1630,7 @@
         <v>45593</v>
       </c>
       <c r="E38" s="3">
-        <v>45579</v>
+        <v>45593</v>
       </c>
       <c r="F38" s="3">
         <v>45576</v>
@@ -1640,7 +1640,7 @@
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="15"/>
+      <c r="B39" s="17"/>
       <c r="C39" s="4" t="s">
         <v>2</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>45607</v>
       </c>
       <c r="E39" s="5">
-        <v>45593</v>
+        <v>45607</v>
       </c>
       <c r="F39" s="5">
         <v>45597</v>
@@ -1658,17 +1658,17 @@
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="15" t="s">
+      <c r="B40" s="17" t="s">
         <v>4</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D40" s="17" t="s">
+      <c r="D40" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E40" s="3">
-        <v>45593</v>
+      <c r="E40" s="13" t="s">
+        <v>11</v>
       </c>
       <c r="F40" s="3">
         <v>45597</v>
@@ -1678,15 +1678,15 @@
       </c>
     </row>
     <row r="41" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="16"/>
+      <c r="B41" s="18"/>
       <c r="C41" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D41" s="18" t="s">
+      <c r="D41" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E41" s="11">
-        <v>45607</v>
+      <c r="E41" s="14" t="s">
+        <v>11</v>
       </c>
       <c r="F41" s="11">
         <v>45604</v>

</xml_diff>

<commit_message>
Aulas do 6, 7, 8 e itinerário
</commit_message>
<xml_diff>
--- a/robotica/Arquivos/img/atividades3tri2024.xlsx
+++ b/robotica/Arquivos/img/atividades3tri2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/23ea03c13864f996/daniloLimaComp/profdanilo.com.br/robotica/Arquivos/img/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="145" documentId="11_F25DC773A252ABDACC10480341994DF85ADE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55CD9438-49CF-4EE4-B84B-9BB86BE73609}"/>
+  <xr:revisionPtr revIDLastSave="205" documentId="11_F25DC773A252ABDACC10480341994DF85ADE58E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07D4FC1B-9629-42D0-902B-240C85224AD3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="6 ano" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="8 ano" sheetId="3" r:id="rId3"/>
     <sheet name="9 ano" sheetId="4" r:id="rId4"/>
     <sheet name="calendário" sheetId="5" r:id="rId5"/>
+    <sheet name="Planilha1" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="18">
   <si>
     <t>Atividade</t>
   </si>
@@ -76,6 +77,24 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>peso</t>
+  </si>
+  <si>
+    <t>Atividade Avaliativa 1</t>
+  </si>
+  <si>
+    <t>Atividade Avaliativa 2</t>
+  </si>
+  <si>
+    <t>Atividade Avaliativa 3</t>
+  </si>
+  <si>
+    <t>Atividade Avaliativa 4</t>
   </si>
 </sst>
 </file>
@@ -133,7 +152,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -276,11 +295,213 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -333,6 +554,72 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1383,8 +1670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C5351AA-6B27-4E59-98AD-11C7A990BB4F}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A30" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+    <sheetView showGridLines="0" topLeftCell="A30" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33:P41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1706,4 +1993,311 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21A1B201-A758-45F2-BA0F-F5FA86CA1216}">
+  <dimension ref="C1:L11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:L11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="8.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="E2" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="27"/>
+      <c r="G2" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="27"/>
+      <c r="I2" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="27"/>
+      <c r="K2" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="26"/>
+    </row>
+    <row r="3" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="19"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C4" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <v>45565</v>
+      </c>
+      <c r="F4" s="28">
+        <v>0.33</v>
+      </c>
+      <c r="G4" s="3">
+        <v>45565</v>
+      </c>
+      <c r="H4" s="28">
+        <v>0.33</v>
+      </c>
+      <c r="I4" s="3">
+        <v>45548</v>
+      </c>
+      <c r="J4" s="28">
+        <v>0.25</v>
+      </c>
+      <c r="K4" s="22">
+        <v>45555</v>
+      </c>
+      <c r="L4" s="35">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="5" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C5" s="39"/>
+      <c r="D5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="5">
+        <v>45579</v>
+      </c>
+      <c r="F5" s="29"/>
+      <c r="G5" s="5">
+        <v>45579</v>
+      </c>
+      <c r="H5" s="29"/>
+      <c r="I5" s="5">
+        <v>45569</v>
+      </c>
+      <c r="J5" s="29"/>
+      <c r="K5" s="23">
+        <v>45562</v>
+      </c>
+      <c r="L5" s="36"/>
+    </row>
+    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C6" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3">
+        <v>45579</v>
+      </c>
+      <c r="F6" s="28">
+        <v>0.33</v>
+      </c>
+      <c r="G6" s="3">
+        <v>45579</v>
+      </c>
+      <c r="H6" s="28">
+        <v>0.33</v>
+      </c>
+      <c r="I6" s="3">
+        <v>45569</v>
+      </c>
+      <c r="J6" s="28">
+        <v>0.25</v>
+      </c>
+      <c r="K6" s="22">
+        <v>45562</v>
+      </c>
+      <c r="L6" s="37">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C7" s="39"/>
+      <c r="D7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="5">
+        <v>45593</v>
+      </c>
+      <c r="F7" s="29"/>
+      <c r="G7" s="5">
+        <v>45593</v>
+      </c>
+      <c r="H7" s="29"/>
+      <c r="I7" s="5">
+        <v>45576</v>
+      </c>
+      <c r="J7" s="29"/>
+      <c r="K7" s="23">
+        <v>45583</v>
+      </c>
+      <c r="L7" s="36"/>
+    </row>
+    <row r="8" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C8" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3">
+        <v>45593</v>
+      </c>
+      <c r="F8" s="28">
+        <v>0.33</v>
+      </c>
+      <c r="G8" s="3">
+        <v>45593</v>
+      </c>
+      <c r="H8" s="28">
+        <v>0.33</v>
+      </c>
+      <c r="I8" s="3">
+        <v>45576</v>
+      </c>
+      <c r="J8" s="28">
+        <v>0.25</v>
+      </c>
+      <c r="K8" s="22">
+        <v>45583</v>
+      </c>
+      <c r="L8" s="37">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="9" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C9" s="39"/>
+      <c r="D9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="5">
+        <v>45607</v>
+      </c>
+      <c r="F9" s="29"/>
+      <c r="G9" s="5">
+        <v>45607</v>
+      </c>
+      <c r="H9" s="29"/>
+      <c r="I9" s="5">
+        <v>45597</v>
+      </c>
+      <c r="J9" s="33"/>
+      <c r="K9" s="23">
+        <v>45590</v>
+      </c>
+      <c r="L9" s="36"/>
+    </row>
+    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C10" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="13"/>
+      <c r="I10" s="22">
+        <v>45597</v>
+      </c>
+      <c r="J10" s="28">
+        <v>0.25</v>
+      </c>
+      <c r="K10" s="31">
+        <v>45590</v>
+      </c>
+      <c r="L10" s="37">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="11" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="40"/>
+      <c r="D11" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="14"/>
+      <c r="I11" s="24">
+        <v>45604</v>
+      </c>
+      <c r="J11" s="34"/>
+      <c r="K11" s="32">
+        <v>45618</v>
+      </c>
+      <c r="L11" s="38"/>
+    </row>
+  </sheetData>
+  <mergeCells count="23">
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="G2:H2"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>